<commit_message>
2023-12-27 DDL 작성 완료
</commit_message>
<xml_diff>
--- a/0.WBS.xlsx
+++ b/0.WBS.xlsx
@@ -286,6 +286,88 @@
     <definedName name="DAYS" hidden="1">#NAME?</definedName>
     <definedName name="DAYS" hidden="1">#NAME?</definedName>
     <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -299,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
   <si>
     <t>기간</t>
   </si>
@@ -1065,6 +1147,9 @@
   <si/>
   <si>
     <t>6.테이블 기술서.xlsx</t>
+  </si>
+  <si>
+    <t>7.DDL.sql</t>
   </si>
 </sst>
 </file>
@@ -19232,7 +19317,7 @@
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="J2" sqref="J2"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L34" sqref="L34"/>
+      <selection pane="bottomRight" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14062500" defaultRowHeight="13.500000" outlineLevelRow="3"/>
@@ -19432,7 +19517,7 @@
       </c>
       <c r="R6" s="378">
         <f ca="1">IF(Q6=100%,0,IF(_xlfn.DAYS(L6,TODAY())=0,0,_xlfn.DAYS(L6,TODAY())))</f>
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S6" s="379"/>
       <c r="U6" s="22"/>
@@ -20502,7 +20587,7 @@
       </c>
       <c r="R26" s="314">
         <f ca="1">IF(Q26=100%,0,IF(_xlfn.DAYS(L26,TODAY())=0,0,_xlfn.DAYS(L26,TODAY())))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S26" s="151"/>
       <c r="T26" s="27"/>
@@ -20816,7 +20901,7 @@
         <v>45286</v>
       </c>
       <c r="P32" s="325">
-        <v>45286</v>
+        <v>45287</v>
       </c>
       <c r="Q32" s="326">
         <v>1</v>
@@ -20826,7 +20911,7 @@
         <v>0</v>
       </c>
       <c r="S32" s="327" t="s">
-        <v>215</v>
+        <v>243</v>
       </c>
       <c r="T32" s="30"/>
       <c r="U32" s="31"/>
@@ -20876,7 +20961,7 @@
       </c>
       <c r="R33" s="314">
         <f ca="1">IF(Q33=100%,0,IF(_xlfn.DAYS(L33,TODAY())=0,0,_xlfn.DAYS(L33,TODAY())))</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S33" s="177"/>
       <c r="T33" s="30"/>
@@ -21760,7 +21845,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{bafaaae3-cfef-ecdd-bafa-aae3cfefecdd}</x14:id>
+          <x14:id>{ce8ede97-bb9a-b9a8-ce8e-de97bb9ab9a8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21774,7 +21859,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3e7e2e67-4b6b-6859-3e7e-2e674b6b6859}</x14:id>
+          <x14:id>{4afa5a13-3f1e-3d2c-4afa-5a133f1e3d2c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21788,7 +21873,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b2f2a2eb-c7e7-e4d5-b2f2-a2ebc7e7e4d5}</x14:id>
+          <x14:id>{c686d69f-b392-b1a7-c686-d69fb392b1a7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21802,7 +21887,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3676266f-4363-6051-3676-266f43636051}</x14:id>
+          <x14:id>{4262521b-3716-3524-4262-521b37163524}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21816,7 +21901,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{aaeabaf3-dfff-eccd-aaea-baf3dfffeccd}</x14:id>
+          <x14:id>{de9ece87-ab8b-a9b8-de9e-ce87ab8ba9b8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21830,7 +21915,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2e6e3e77-5b7b-6849-2e6e-3e775b7b6849}</x14:id>
+          <x14:id>{5a1a4a53-2f8f-2d3c-5a1a-4a532f8f2d3c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21844,7 +21929,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{a2e2b2fb-d7f7-e4c5-a2e2-b2fbd7f7e4c5}</x14:id>
+          <x14:id>{d696c68f-a383-a1b6-d696-c68fa383a1b6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21858,7 +21943,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2666367f-5373-6141-2666-367f53736141}</x14:id>
+          <x14:id>{521242cb-2717-2534-5212-42cb27172534}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21872,7 +21957,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9ada8ac3-efcf-ecfd-9ada-8ac3efcfecfd}</x14:id>
+          <x14:id>{eeaefeb7-9bb8-9988-eeae-feb79bb89988}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21886,7 +21971,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1e5e5e47-6b4b-6879-1e5e-5e476b4b6879}</x14:id>
+          <x14:id>{6a2a7a33-1f3c-1d1c-6a2a-7a331f3c1d1c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21899,7 +21984,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{bafaaae3-cfef-ecdd-bafa-aae3cfefecdd}">
+          <x14:cfRule type="dataBar" id="{ce8ede97-bb9a-b9a8-ce8e-de97bb9ab9a8}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -21910,7 +21995,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3e7e2e67-4b6b-6859-3e7e-2e674b6b6859}">
+          <x14:cfRule type="dataBar" id="{4afa5a13-3f1e-3d2c-4afa-5a133f1e3d2c}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -21921,7 +22006,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b2f2a2eb-c7e7-e4d5-b2f2-a2ebc7e7e4d5}">
+          <x14:cfRule type="dataBar" id="{c686d69f-b392-b1a7-c686-d69fb392b1a7}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -21932,7 +22017,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3676266f-4363-6051-3676-266f43636051}">
+          <x14:cfRule type="dataBar" id="{4262521b-3716-3524-4262-521b37163524}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -21943,7 +22028,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{aaeabaf3-dfff-eccd-aaea-baf3dfffeccd}">
+          <x14:cfRule type="dataBar" id="{de9ece87-ab8b-a9b8-de9e-ce87ab8ba9b8}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -21954,7 +22039,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2e6e3e77-5b7b-6849-2e6e-3e775b7b6849}">
+          <x14:cfRule type="dataBar" id="{5a1a4a53-2f8f-2d3c-5a1a-4a532f8f2d3c}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -21965,7 +22050,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{a2e2b2fb-d7f7-e4c5-a2e2-b2fbd7f7e4c5}">
+          <x14:cfRule type="dataBar" id="{d696c68f-a383-a1b6-d696-c68fa383a1b6}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -21976,7 +22061,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2666367f-5373-6141-2666-367f53736141}">
+          <x14:cfRule type="dataBar" id="{521242cb-2717-2534-5212-42cb27172534}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -21987,7 +22072,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9ada8ac3-efcf-ecfd-9ada-8ac3efcfecfd}">
+          <x14:cfRule type="dataBar" id="{eeaefeb7-9bb8-9988-eeae-feb79bb89988}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -21998,7 +22083,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1e5e5e47-6b4b-6879-1e5e-5e476b4b6879}">
+          <x14:cfRule type="dataBar" id="{6a2a7a33-1f3c-1d1c-6a2a-7a331f3c1d1c}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
2024-01-03 API 설계서 완성
</commit_message>
<xml_diff>
--- a/0.WBS.xlsx
+++ b/0.WBS.xlsx
@@ -450,6 +450,252 @@
     <definedName name="DAYS" hidden="1">#NAME?</definedName>
     <definedName name="DAYS" hidden="1">#NAME?</definedName>
     <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -463,7 +709,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="254">
   <si>
     <t>기간</t>
   </si>
@@ -1259,6 +1505,9 @@
   </si>
   <si>
     <t>8.기능정리.xlsx</t>
+  </si>
+  <si>
+    <t>9.API 설계서.json</t>
   </si>
 </sst>
 </file>
@@ -19422,11 +19671,11 @@
   <dimension ref="B2:AD63"/>
   <sheetViews>
     <sheetView topLeftCell="A2" showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="9" ySplit="5" topLeftCell="J25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="5" topLeftCell="J22" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="J2" sqref="J2"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="O36" sqref="O36"/>
+      <selection pane="bottomRight" activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14062500" defaultRowHeight="13.500000" outlineLevelRow="3"/>
@@ -19626,7 +19875,7 @@
       </c>
       <c r="R6" s="378">
         <f ca="1">IF(Q6=100%,0,IF(_xlfn.DAYS(L6,TODAY())=0,0,_xlfn.DAYS(L6,TODAY())))</f>
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="S6" s="379"/>
       <c r="U6" s="22"/>
@@ -20672,13 +20921,13 @@
       <c r="I26" s="140"/>
       <c r="J26" s="368" t="str">
         <f>CONCATENATE(NETWORKDAYS(K26,L26),"일")</f>
-        <v>10일</v>
+        <v>15일</v>
       </c>
       <c r="K26" s="144">
         <v>45278</v>
       </c>
       <c r="L26" s="144">
-        <v>45289</v>
+        <v>45298</v>
       </c>
       <c r="M26" s="144" t="s">
         <v>50</v>
@@ -20692,11 +20941,11 @@
       <c r="P26" s="144"/>
       <c r="Q26" s="145">
         <f>(SUM(Q27,Q28,Q33)/COUNT(Q27,Q28,Q33))</f>
-        <v>0.777777777777778</v>
+        <v>0.888888888888889</v>
       </c>
       <c r="R26" s="314">
         <f ca="1">IF(Q26=100%,0,IF(_xlfn.DAYS(L26,TODAY())=0,0,_xlfn.DAYS(L26,TODAY())))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S26" s="151"/>
       <c r="T26" s="27"/>
@@ -21067,11 +21316,11 @@
       </c>
       <c r="Q33" s="307">
         <f>SUM(Q34:Q36)/COUNT(Q34:Q36)</f>
-        <v>0.333333333333333</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="R33" s="314">
         <f ca="1">IF(Q33=100%,0,IF(_xlfn.DAYS(L33,TODAY())=0,0,_xlfn.DAYS(L33,TODAY())))</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="S33" s="177"/>
       <c r="T33" s="30"/>
@@ -21168,17 +21417,17 @@
         <v>45288</v>
       </c>
       <c r="P35" s="325">
-        <v>45289</v>
+        <v>45294</v>
       </c>
       <c r="Q35" s="326">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R35" s="314">
         <f ca="1">IF(Q35=100%,0,IF(_xlfn.DAYS(L35,TODAY())=0,0,_xlfn.DAYS(L35,TODAY())))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S35" s="327" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="T35" s="30"/>
       <c r="U35" s="31"/>
@@ -21205,10 +21454,10 @@
       <c r="I36" s="319"/>
       <c r="J36" s="365" t="str">
         <f>CONCATENATE(_xlfn.DAYS(L36,K36),"일")</f>
-        <v>5일</v>
-      </c>
-      <c r="K36" s="323">
-        <v>45293</v>
+        <v>3일</v>
+      </c>
+      <c r="K36" s="325">
+        <v>45295</v>
       </c>
       <c r="L36" s="323">
         <v>45298</v>
@@ -21217,14 +21466,16 @@
       <c r="N36" s="324" t="s">
         <v>167</v>
       </c>
-      <c r="O36" s="325"/>
+      <c r="O36" s="325">
+        <v>45295</v>
+      </c>
       <c r="P36" s="325"/>
       <c r="Q36" s="326">
         <v>0</v>
       </c>
       <c r="R36" s="314">
         <f ca="1">IF(Q36=100%,0,IF(_xlfn.DAYS(L36,TODAY())=0,0,_xlfn.DAYS(L36,TODAY())))</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="S36" s="327" t="s">
         <v>250</v>
@@ -21981,7 +22232,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2363337a-5677-7544-2363-337a56777544}</x14:id>
+          <x14:id>{98d888c1-eddc-effe-98d8-88c1eddceffe}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21995,7 +22246,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{a7e7b7fe-d2f3-f1cb-a7e7-b7fed2f3f1cb}</x14:id>
+          <x14:id>{1c5c9c45-6958-6b7a-1c5c-9c4569586b7a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22009,7 +22260,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2b6b3b72-5e7f-7d4c-2b6b-3b725e7f7d4c}</x14:id>
+          <x14:id>{9ede8ec9-e5d4-e7f6-9ede-8ec9e5d4e7f6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22023,7 +22274,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{afefbff6-dafb-f9c8-afef-bff6dafbf9c8}</x14:id>
+          <x14:id>{1454044d-6157-6372-1454-044d61576372}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22037,7 +22288,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3373236a-4667-7554-3373-236a46677554}</x14:id>
+          <x14:id>{88c898d1-fdcd-ffee-88c8-98d1fdcdffee}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22051,7 +22302,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b7f7a7ee-c2e3-f1da-b7f7-a7eec2e3f1da}</x14:id>
+          <x14:id>{3c4c1c55-7949-7b6a-3c4c-1c5579497b6a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22065,7 +22316,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3b7b2b62-4e6f-7d5c-3b7b-2b624e6f7d5c}</x14:id>
+          <x14:id>{8fcf9fd9-f5c5-f7e6-8fcf-9fd9f5c5f7e6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22079,7 +22330,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{bfffafe6-caeb-f9d8-bfff-afe6caebf9d8}</x14:id>
+          <x14:id>{a444145d-7141-7362-a444-145d71417362}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22093,7 +22344,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f343135a-7657-7564-f343-135a76577564}</x14:id>
+          <x14:id>{b8f8a8e1-cdfe-cfde-b8f8-a8e1cdfecfde}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22107,7 +22358,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{87c797de-f2d3-f1ed-87c7-97def2d3f1ed}</x14:id>
+          <x14:id>{3c7c2c65-497a-4b5a-3c7c-2c65497a4b5a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -22120,7 +22371,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2363337a-5677-7544-2363-337a56777544}">
+          <x14:cfRule type="dataBar" id="{98d888c1-eddc-effe-98d8-88c1eddceffe}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -22131,7 +22382,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{a7e7b7fe-d2f3-f1cb-a7e7-b7fed2f3f1cb}">
+          <x14:cfRule type="dataBar" id="{1c5c9c45-6958-6b7a-1c5c-9c4569586b7a}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -22142,7 +22393,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2b6b3b72-5e7f-7d4c-2b6b-3b725e7f7d4c}">
+          <x14:cfRule type="dataBar" id="{9ede8ec9-e5d4-e7f6-9ede-8ec9e5d4e7f6}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -22153,7 +22404,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{afefbff6-dafb-f9c8-afef-bff6dafbf9c8}">
+          <x14:cfRule type="dataBar" id="{1454044d-6157-6372-1454-044d61576372}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -22164,7 +22415,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3373236a-4667-7554-3373-236a46677554}">
+          <x14:cfRule type="dataBar" id="{88c898d1-fdcd-ffee-88c8-98d1fdcdffee}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -22175,7 +22426,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b7f7a7ee-c2e3-f1da-b7f7-a7eec2e3f1da}">
+          <x14:cfRule type="dataBar" id="{3c4c1c55-7949-7b6a-3c4c-1c5579497b6a}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -22186,7 +22437,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3b7b2b62-4e6f-7d5c-3b7b-2b624e6f7d5c}">
+          <x14:cfRule type="dataBar" id="{8fcf9fd9-f5c5-f7e6-8fcf-9fd9f5c5f7e6}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -22197,7 +22448,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{bfffafe6-caeb-f9d8-bfff-afe6caebf9d8}">
+          <x14:cfRule type="dataBar" id="{a444145d-7141-7362-a444-145d71417362}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -22208,7 +22459,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f343135a-7657-7564-f343-135a76577564}">
+          <x14:cfRule type="dataBar" id="{b8f8a8e1-cdfe-cfde-b8f8-a8e1cdfecfde}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -22219,7 +22470,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{87c797de-f2d3-f1ed-87c7-97def2d3f1ed}">
+          <x14:cfRule type="dataBar" id="{3c7c2c65-497a-4b5a-3c7c-2c65497a4b5a}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
2024-01-23 Logging  정리 & Login 로직 80% 완성
</commit_message>
<xml_diff>
--- a/0.WBS.xlsx
+++ b/0.WBS.xlsx
@@ -17,6 +17,104 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">WBS!$C$19:$S$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">history!$A$1:$H$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">WBS!$A$2:$S$56</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
+    <definedName name="DAYS" hidden="1">#NAME?</definedName>
     <definedName name="DAYS" hidden="1">#NAME?</definedName>
     <definedName name="DAYS" hidden="1">#NAME?</definedName>
     <definedName name="DAYS" hidden="1">#NAME?</definedName>
@@ -17402,7 +17500,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -17437,7 +17535,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -17647,7 +17745,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -17682,7 +17780,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -18172,7 +18270,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -18207,7 +18305,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -18557,7 +18655,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -18592,7 +18690,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -18802,7 +18900,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -18837,7 +18935,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -19327,7 +19425,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -19362,7 +19460,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13602335" y="11287125"/>
+          <a:off x="13597890" y="11287125"/>
           <a:ext cx="0" cy="246380"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
@@ -20863,11 +20961,11 @@
   <dimension ref="B2:AD72"/>
   <sheetViews>
     <sheetView topLeftCell="A2" showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="9" ySplit="5" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="5" topLeftCell="J40" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="J2" sqref="J2"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="O47" sqref="O47"/>
+      <selection pane="bottomRight" activeCell="H50" sqref="H50:I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14062500" defaultRowHeight="13.500000" outlineLevelRow="3"/>
@@ -21067,7 +21165,7 @@
       </c>
       <c r="R6" s="378">
         <f ca="1">IF(Q6=100%,0,IF(_xlfn.DAYS(L6,TODAY())=0,0,_xlfn.DAYS(L6,TODAY())))</f>
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S6" s="379"/>
       <c r="U6" s="22"/>
@@ -23169,9 +23267,11 @@
       <c r="O46" s="325">
         <v>45310</v>
       </c>
-      <c r="P46" s="325"/>
+      <c r="P46" s="325">
+        <v>45310</v>
+      </c>
       <c r="Q46" s="326">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46" s="314">
         <f ca="1">IF(Q46=100%,0,IF(_xlfn.DAYS(L46,TODAY())=0,0,_xlfn.DAYS(L46,TODAY())))</f>
@@ -23222,7 +23322,7 @@
       </c>
       <c r="R47" s="314">
         <f ca="1">IF(Q47=100%,0,IF(_xlfn.DAYS(L47,TODAY())=0,0,_xlfn.DAYS(L47,TODAY())))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S47" s="177"/>
       <c r="T47" s="30"/>
@@ -23269,7 +23369,7 @@
       </c>
       <c r="R48" s="314">
         <f ca="1">IF(Q48=100%,0,IF(_xlfn.DAYS(L48,TODAY())=0,0,_xlfn.DAYS(L48,TODAY())))</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="S48" s="177"/>
       <c r="T48" s="30"/>
@@ -23651,25 +23751,16 @@
     </row>
     <row r="58" spans="2:22" outlineLevel="1">
       <c r="B58" s="32"/>
-      <c r="C58" s="16"/>
       <c r="D58" s="32"/>
       <c r="E58" s="32"/>
       <c r="F58" s="32"/>
       <c r="G58" s="32"/>
       <c r="H58" s="32"/>
       <c r="I58" s="32"/>
-      <c r="J58" s="15"/>
       <c r="K58" s="32"/>
-      <c r="L58" s="35"/>
       <c r="M58" s="32"/>
       <c r="N58" s="32"/>
-      <c r="O58" s="35"/>
-      <c r="P58" s="35"/>
-      <c r="Q58" s="36"/>
-      <c r="R58" s="34"/>
-      <c r="S58" s="37"/>
       <c r="T58" s="32"/>
-      <c r="U58" s="20"/>
       <c r="V58" s="32"/>
     </row>
     <row r="59" spans="2:22">
@@ -23775,30 +23866,18 @@
       <c r="T64" s="32"/>
       <c r="V64" s="32"/>
     </row>
-    <row r="65" spans="2:22">
-      <c r="B65" s="15"/>
+    <row r="65" spans="3:21">
       <c r="C65" s="32"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="15"/>
-      <c r="I65" s="16"/>
       <c r="J65" s="32"/>
-      <c r="K65" s="35"/>
       <c r="L65" s="32"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="35"/>
       <c r="O65" s="32"/>
       <c r="P65" s="32"/>
       <c r="Q65" s="32"/>
       <c r="R65" s="33"/>
       <c r="S65" s="32"/>
-      <c r="T65" s="15"/>
       <c r="U65" s="32"/>
-      <c r="V65" s="15"/>
     </row>
-    <row r="66" spans="2:22">
+    <row r="66" spans="3:21">
       <c r="C66" s="32"/>
       <c r="J66" s="32"/>
       <c r="L66" s="32"/>
@@ -23808,7 +23887,7 @@
       <c r="S66" s="32"/>
       <c r="U66" s="32"/>
     </row>
-    <row r="67" spans="2:22">
+    <row r="67" spans="3:21">
       <c r="C67" s="32"/>
       <c r="J67" s="32"/>
       <c r="L67" s="32"/>
@@ -23819,7 +23898,7 @@
       <c r="S67" s="32"/>
       <c r="U67" s="32"/>
     </row>
-    <row r="68" spans="2:22">
+    <row r="68" spans="3:21">
       <c r="C68" s="29"/>
       <c r="J68" s="29"/>
       <c r="L68" s="29"/>
@@ -23830,7 +23909,7 @@
       <c r="S68" s="29"/>
       <c r="U68" s="29"/>
     </row>
-    <row r="69" spans="2:22">
+    <row r="69" spans="3:21">
       <c r="C69" s="32"/>
       <c r="J69" s="32"/>
       <c r="L69" s="32"/>
@@ -23841,7 +23920,7 @@
       <c r="S69" s="32"/>
       <c r="U69" s="32"/>
     </row>
-    <row r="70" spans="2:22">
+    <row r="70" spans="3:21">
       <c r="C70" s="32"/>
       <c r="J70" s="32"/>
       <c r="L70" s="32"/>
@@ -23852,8 +23931,7 @@
       <c r="S70" s="32"/>
       <c r="U70" s="32"/>
     </row>
-    <row r="71" spans="2:22">
-      <c r="C71" s="16"/>
+    <row r="71" spans="3:21">
       <c r="J71" s="32"/>
       <c r="L71" s="32"/>
       <c r="O71" s="32"/>
@@ -23862,16 +23940,6 @@
       <c r="R71" s="32"/>
       <c r="S71" s="32"/>
       <c r="U71" s="32"/>
-    </row>
-    <row r="72" spans="2:22">
-      <c r="J72" s="15"/>
-      <c r="L72" s="35"/>
-      <c r="O72" s="35"/>
-      <c r="P72" s="35"/>
-      <c r="Q72" s="36"/>
-      <c r="R72" s="34"/>
-      <c r="S72" s="37"/>
-      <c r="U72" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="47">
@@ -23933,7 +24001,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{cb8bdb92-be8d-9dac-cb8b-db92be8d9dac}</x14:id>
+          <x14:id>{3a7a2a63-4f6f-6c5d-3a7a-2a634f6f6c5d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -23947,7 +24015,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4faf5f16-3af9-1928-4faf-5f163af91928}</x14:id>
+          <x14:id>{befeaee7-cbeb-e8d9-befe-aee7cbebe8d9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -23961,7 +24029,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{d393c38a-a695-95b4-d393-c38aa69595b4}</x14:id>
+          <x14:id>{2262327b-5777-6445-2262-327b57776445}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -23975,7 +24043,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5717479e-2211-113a-5717-479e2211113a}</x14:id>
+          <x14:id>{a6e6b6ff-d3f3-e8c1-a6e6-b6ffd3f3e8c1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -23989,7 +24057,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{db9bcb82-ae9d-9dbc-db9b-cb82ae9d9dbc}</x14:id>
+          <x14:id>{2a6a3a73-5f7f-6c4d-2a6a-3a735f7f6c4d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24003,7 +24071,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5f1f4f06-2a19-1938-5f1f-4f062a191938}</x14:id>
+          <x14:id>{aeeebef7-dbfb-e8c9-aeee-bef7dbfbe8c9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24017,7 +24085,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{e3a3f3ba-96a5-9584-e3a3-f3ba96a59584}</x14:id>
+          <x14:id>{1252c24b-6747-6475-1252-c24b67476475}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24031,7 +24099,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6727773e-1221-11dd-6727-773e122111dd}</x14:id>
+          <x14:id>{96d686cf-e3c3-eff1-96d6-86cfe3c3eff1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24045,7 +24113,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ebabfbb2-9eaf-bd8c-ebab-fbb29eafbd8c}</x14:id>
+          <x14:id>{febeeea7-8bab-a899-febe-eea78baba899}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24059,7 +24127,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6f2f7f36-1a2b-39e8-6f2f-7f361a2b39e8}</x14:id>
+          <x14:id>{7a3a6a23-4f2f-2c1d-7a3a-6a234f2f2c1d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24073,7 +24141,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{e3a3f3ba-96a7-b584-e3a3-f3ba96a7b584}</x14:id>
+          <x14:id>{f6b6e6af-83a3-a591-f6b6-e6af83a3a591}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24087,7 +24155,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6727773e-1223-3174-6727-773e12233174}</x14:id>
+          <x14:id>{7232622b-d727-2415-7232-622bd7272415}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24101,7 +24169,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{fbbbeba2-8ebf-bd9c-fbbb-eba28ebfbd9c}</x14:id>
+          <x14:id>{eeaefeb7-9bbb-a889-eeae-feb79bbba889}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24115,7 +24183,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7f3f6f26-2a3b-3918-7f3f-6f262a3b3918}</x14:id>
+          <x14:id>{6a2a7a33-1f3f-2c8d-6a2a-7a331f3f2c8d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24129,7 +24197,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f3b3e3aa-86b7-b594-f3b3-e3aa86b7b594}</x14:id>
+          <x14:id>{e6a6f6bf-93b3-a481-e6a6-f6bf93b3a481}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24143,7 +24211,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7737672e-b233-3115-7737-672eb2333115}</x14:id>
+          <x14:id>{6222723b-1737-2415-6222-723b17372415}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24157,7 +24225,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{cb8bdb92-be8f-bdac-cb8b-db92be8fbdac}</x14:id>
+          <x14:id>{de9ece87-ab8b-a8b9-de9e-ce87ab8ba8b9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24171,7 +24239,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4f0f5f16-3a9b-3928-4f0f-5f163a9b3928}</x14:id>
+          <x14:id>{5a1a4ac3-2f9f-2c3d-5a1a-4ac32f9f2c3d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24185,7 +24253,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2767377e-5263-7148-2767-377e52637148}</x14:id>
+          <x14:id>{bbfbabe2-ceee-eddc-bbfb-abe2ceeeeddc}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24199,7 +24267,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{a3e3b3fa-d6e7-f5c4-a3e3-b3fad6e7f5c4}</x14:id>
+          <x14:id>{3f7f2f66-4a6a-6958-3f7f-2f664a6a6958}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24213,7 +24281,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2f6f3f76-5a6b-7948-2f6f-3f765a6b7948}</x14:id>
+          <x14:id>{b3f3a3ea-c6e6-e5d4-b3f3-a3eac6e6e5d4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24227,7 +24295,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{abebbbf2-deef-fdcc-abeb-bbf2deeffdcc}</x14:id>
+          <x14:id>{3777276e-4262-6151-3777-276e42626151}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24241,7 +24309,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3777276e-4273-7159-3777-276e42737159}</x14:id>
+          <x14:id>{abebbbf2-defe-edcc-abeb-bbf2defeedcc}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24255,7 +24323,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b3f3a3ea-c6f7-f5d4-b3f3-a3eac6f7f5d4}</x14:id>
+          <x14:id>{2f6f3f76-5a7a-6948-2f6f-3f765a7a6948}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24269,7 +24337,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3f7f2f66-4a7b-7958-3f7f-2f664a7b7958}</x14:id>
+          <x14:id>{a3e3b3fa-d6f6-e5c4-a3e3-b3fad6f6e5c4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24283,7 +24351,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{bbfbabe2-ceff-fddc-bbfb-abe2cefffddc}</x14:id>
+          <x14:id>{2767377e-5272-6140-2767-377e52726140}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24297,7 +24365,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0747175e-7243-716e-0747-175e7243716e}</x14:id>
+          <x14:id>{9bdb8bc2-eece-edfc-9bdb-8bc2eeceedfc}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24311,7 +24379,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{83c393da-f6c7-f5e4-83c3-93daf6c7f5e4}</x14:id>
+          <x14:id>{1f5f1f46-6a4a-6978-1f5f-1f466a4a6978}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24325,7 +24393,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6222723b-1726-3435-6222-723b17263435}</x14:id>
+          <x14:id>{7737672e-9222-211d-7737-672e9222211d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24339,7 +24407,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{e6a6f6bf-93a2-bc81-e6a6-f6bf93a2bc81}</x14:id>
+          <x14:id>{f3b3e3aa-86a6-a594-f3b3-e3aa86a6a594}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24353,7 +24421,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6a2a7a33-1f2e-3cad-6a2a-7a331f2e3cad}</x14:id>
+          <x14:id>{7f3f6f26-0a2a-2918-7f3f-6f260a2a2918}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24367,7 +24435,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{eeaefeb7-9baa-b889-eeae-feb79baab889}</x14:id>
+          <x14:id>{fbbbeba2-8eae-ad9c-fbbb-eba28eaead9c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24381,7 +24449,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7232622b-f736-3415-7232-622bf7363415}</x14:id>
+          <x14:id>{6727773e-1232-215c-6727-773e1232215c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24395,7 +24463,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f6b6e6af-83b2-bd91-f6b6-e6af83b2bd91}</x14:id>
+          <x14:id>{e3a3f3ba-96b6-a584-e3a3-f3ba96b6a584}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24409,7 +24477,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7a3a6a23-6f3e-3c1d-7a3a-6a236f3e3c1d}</x14:id>
+          <x14:id>{6f2f7f36-1a3a-29c8-6f2f-7f361a3a29c8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24423,7 +24491,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{febeeea7-8bba-b899-febe-eea78bbab899}</x14:id>
+          <x14:id>{ebabfbb2-9ebe-ad8c-ebab-fbb29ebead8c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24437,7 +24505,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{42d2521b-3746-3425-42d2-521b37463425}</x14:id>
+          <x14:id>{5717471e-2242-213b-5717-471e2242213b}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24451,7 +24519,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{c686d69f-b382-baa1-c686-d69fb382baa1}</x14:id>
+          <x14:id>{d393c38a-a686-a5b4-d393-c38aa686a5b4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -24464,7 +24532,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{cb8bdb92-be8d-9dac-cb8b-db92be8d9dac}">
+          <x14:cfRule type="dataBar" id="{3a7a2a63-4f6f-6c5d-3a7a-2a634f6f6c5d}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24475,7 +24543,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4faf5f16-3af9-1928-4faf-5f163af91928}">
+          <x14:cfRule type="dataBar" id="{befeaee7-cbeb-e8d9-befe-aee7cbebe8d9}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24486,7 +24554,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{d393c38a-a695-95b4-d393-c38aa69595b4}">
+          <x14:cfRule type="dataBar" id="{2262327b-5777-6445-2262-327b57776445}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24497,7 +24565,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5717479e-2211-113a-5717-479e2211113a}">
+          <x14:cfRule type="dataBar" id="{a6e6b6ff-d3f3-e8c1-a6e6-b6ffd3f3e8c1}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24508,7 +24576,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{db9bcb82-ae9d-9dbc-db9b-cb82ae9d9dbc}">
+          <x14:cfRule type="dataBar" id="{2a6a3a73-5f7f-6c4d-2a6a-3a735f7f6c4d}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24519,7 +24587,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5f1f4f06-2a19-1938-5f1f-4f062a191938}">
+          <x14:cfRule type="dataBar" id="{aeeebef7-dbfb-e8c9-aeee-bef7dbfbe8c9}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24530,7 +24598,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{e3a3f3ba-96a5-9584-e3a3-f3ba96a59584}">
+          <x14:cfRule type="dataBar" id="{1252c24b-6747-6475-1252-c24b67476475}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24541,7 +24609,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6727773e-1221-11dd-6727-773e122111dd}">
+          <x14:cfRule type="dataBar" id="{96d686cf-e3c3-eff1-96d6-86cfe3c3eff1}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24552,7 +24620,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ebabfbb2-9eaf-bd8c-ebab-fbb29eafbd8c}">
+          <x14:cfRule type="dataBar" id="{febeeea7-8bab-a899-febe-eea78baba899}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24563,7 +24631,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6f2f7f36-1a2b-39e8-6f2f-7f361a2b39e8}">
+          <x14:cfRule type="dataBar" id="{7a3a6a23-4f2f-2c1d-7a3a-6a234f2f2c1d}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24574,7 +24642,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{e3a3f3ba-96a7-b584-e3a3-f3ba96a7b584}">
+          <x14:cfRule type="dataBar" id="{f6b6e6af-83a3-a591-f6b6-e6af83a3a591}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24585,7 +24653,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6727773e-1223-3174-6727-773e12233174}">
+          <x14:cfRule type="dataBar" id="{7232622b-d727-2415-7232-622bd7272415}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24596,7 +24664,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{fbbbeba2-8ebf-bd9c-fbbb-eba28ebfbd9c}">
+          <x14:cfRule type="dataBar" id="{eeaefeb7-9bbb-a889-eeae-feb79bbba889}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24607,7 +24675,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7f3f6f26-2a3b-3918-7f3f-6f262a3b3918}">
+          <x14:cfRule type="dataBar" id="{6a2a7a33-1f3f-2c8d-6a2a-7a331f3f2c8d}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24618,7 +24686,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f3b3e3aa-86b7-b594-f3b3-e3aa86b7b594}">
+          <x14:cfRule type="dataBar" id="{e6a6f6bf-93b3-a481-e6a6-f6bf93b3a481}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24629,7 +24697,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7737672e-b233-3115-7737-672eb2333115}">
+          <x14:cfRule type="dataBar" id="{6222723b-1737-2415-6222-723b17372415}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24640,7 +24708,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{cb8bdb92-be8f-bdac-cb8b-db92be8fbdac}">
+          <x14:cfRule type="dataBar" id="{de9ece87-ab8b-a8b9-de9e-ce87ab8ba8b9}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24651,7 +24719,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4f0f5f16-3a9b-3928-4f0f-5f163a9b3928}">
+          <x14:cfRule type="dataBar" id="{5a1a4ac3-2f9f-2c3d-5a1a-4ac32f9f2c3d}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24662,7 +24730,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2767377e-5263-7148-2767-377e52637148}">
+          <x14:cfRule type="dataBar" id="{bbfbabe2-ceee-eddc-bbfb-abe2ceeeeddc}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24673,7 +24741,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{a3e3b3fa-d6e7-f5c4-a3e3-b3fad6e7f5c4}">
+          <x14:cfRule type="dataBar" id="{3f7f2f66-4a6a-6958-3f7f-2f664a6a6958}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24684,7 +24752,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2f6f3f76-5a6b-7948-2f6f-3f765a6b7948}">
+          <x14:cfRule type="dataBar" id="{b3f3a3ea-c6e6-e5d4-b3f3-a3eac6e6e5d4}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24695,7 +24763,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{abebbbf2-deef-fdcc-abeb-bbf2deeffdcc}">
+          <x14:cfRule type="dataBar" id="{3777276e-4262-6151-3777-276e42626151}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24706,7 +24774,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3777276e-4273-7159-3777-276e42737159}">
+          <x14:cfRule type="dataBar" id="{abebbbf2-defe-edcc-abeb-bbf2defeedcc}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24717,7 +24785,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b3f3a3ea-c6f7-f5d4-b3f3-a3eac6f7f5d4}">
+          <x14:cfRule type="dataBar" id="{2f6f3f76-5a7a-6948-2f6f-3f765a7a6948}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24728,7 +24796,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3f7f2f66-4a7b-7958-3f7f-2f664a7b7958}">
+          <x14:cfRule type="dataBar" id="{a3e3b3fa-d6f6-e5c4-a3e3-b3fad6f6e5c4}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24739,7 +24807,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{bbfbabe2-ceff-fddc-bbfb-abe2cefffddc}">
+          <x14:cfRule type="dataBar" id="{2767377e-5272-6140-2767-377e52726140}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24750,7 +24818,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0747175e-7243-716e-0747-175e7243716e}">
+          <x14:cfRule type="dataBar" id="{9bdb8bc2-eece-edfc-9bdb-8bc2eeceedfc}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24761,7 +24829,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{83c393da-f6c7-f5e4-83c3-93daf6c7f5e4}">
+          <x14:cfRule type="dataBar" id="{1f5f1f46-6a4a-6978-1f5f-1f466a4a6978}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24772,7 +24840,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6222723b-1726-3435-6222-723b17263435}">
+          <x14:cfRule type="dataBar" id="{7737672e-9222-211d-7737-672e9222211d}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24783,7 +24851,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{e6a6f6bf-93a2-bc81-e6a6-f6bf93a2bc81}">
+          <x14:cfRule type="dataBar" id="{f3b3e3aa-86a6-a594-f3b3-e3aa86a6a594}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24794,7 +24862,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6a2a7a33-1f2e-3cad-6a2a-7a331f2e3cad}">
+          <x14:cfRule type="dataBar" id="{7f3f6f26-0a2a-2918-7f3f-6f260a2a2918}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24805,7 +24873,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{eeaefeb7-9baa-b889-eeae-feb79baab889}">
+          <x14:cfRule type="dataBar" id="{fbbbeba2-8eae-ad9c-fbbb-eba28eaead9c}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24816,7 +24884,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7232622b-f736-3415-7232-622bf7363415}">
+          <x14:cfRule type="dataBar" id="{6727773e-1232-215c-6727-773e1232215c}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24827,7 +24895,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f6b6e6af-83b2-bd91-f6b6-e6af83b2bd91}">
+          <x14:cfRule type="dataBar" id="{e3a3f3ba-96b6-a584-e3a3-f3ba96b6a584}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24838,7 +24906,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7a3a6a23-6f3e-3c1d-7a3a-6a236f3e3c1d}">
+          <x14:cfRule type="dataBar" id="{6f2f7f36-1a3a-29c8-6f2f-7f361a3a29c8}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24849,7 +24917,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{febeeea7-8bba-b899-febe-eea78bbab899}">
+          <x14:cfRule type="dataBar" id="{ebabfbb2-9ebe-ad8c-ebab-fbb29ebead8c}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24860,7 +24928,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{42d2521b-3746-3425-42d2-521b37463425}">
+          <x14:cfRule type="dataBar" id="{5717471e-2242-213b-5717-471e2242213b}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -24871,7 +24939,7 @@
           </x14:cfRule>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{c686d69f-b382-baa1-c686-d69fb382baa1}">
+          <x14:cfRule type="dataBar" id="{d393c38a-a686-a5b4-d393-c38aa686a5b4}">
             <x14:dataBar minLength="0" maxLength="100" border="1" gradient="1">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>